<commit_message>
Added login by user feature
</commit_message>
<xml_diff>
--- a/Design/Db_tables.xlsx
+++ b/Design/Db_tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>User_name</t>
   </si>
@@ -24,9 +24,6 @@
     <t>User_password(SALT included)</t>
   </si>
   <si>
-    <t>PictureSignature</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -142,6 +139,12 @@
   </si>
   <si>
     <t>number of retries before locked</t>
+  </si>
+  <si>
+    <t>User_pictures</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
   </si>
 </sst>
 </file>
@@ -178,15 +181,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -274,14 +283,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -296,6 +341,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -602,266 +651,268 @@
     <col min="3" max="3" width="26.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="E3" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1"/>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1">
+      <c r="A12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1">
-      <c r="A7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1"/>
-    <row r="10" spans="1:3" ht="15">
-      <c r="A10" s="2" t="s">
+      <c r="C12" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1"/>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1">
-      <c r="A13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1"/>
-    <row r="16" spans="1:3" ht="15">
-      <c r="A16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>12</v>
+      <c r="B17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="15">
+      <c r="A23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="5" t="s">
+      <c r="B24" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15">
-      <c r="A26" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>34</v>
-      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15">
+      <c r="A25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickBot="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>